<commit_message>
Updated Gantt chart 1st July
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37FD3CC-1E98-4418-B00F-094DCEC68B6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B25A623-B81A-485D-9F37-4EA9B6B85836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>Prepare final video presentation</t>
   </si>
   <si>
-    <t>Set up unit tests for authentication functions implemented (Mocha, Chai)</t>
-  </si>
-  <si>
     <t>Development - 
 Authentication</t>
   </si>
@@ -203,9 +200,6 @@
     <t>routing</t>
   </si>
   <si>
-    <t>unit tests (Mocha, Chai)</t>
-  </si>
-  <si>
     <t>create mock DB objects</t>
   </si>
   <si>
@@ -307,6 +301,12 @@
   </si>
   <si>
     <t>1-17</t>
+  </si>
+  <si>
+    <t>Set up unit tests for authentication functions implemented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit tests </t>
   </si>
 </sst>
 </file>
@@ -322,7 +322,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -468,14 +474,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,12 +497,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,7 +827,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -830,13 +837,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="15">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="10">
         <v>26</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
@@ -846,7 +853,7 @@
       <c r="B3" s="3">
         <v>4</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
@@ -856,7 +863,7 @@
       <c r="B4" s="3">
         <v>9</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="13">
         <v>2</v>
       </c>
     </row>
@@ -868,8 +875,8 @@
       <c r="B5" s="3">
         <v>7</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>89</v>
+      <c r="C5" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -880,8 +887,8 @@
       <c r="B6" s="3">
         <v>7</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>89</v>
+      <c r="C6" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -892,8 +899,8 @@
       <c r="B7" s="3">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>89</v>
+      <c r="C7" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -904,8 +911,8 @@
       <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>89</v>
+      <c r="C8" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -916,8 +923,8 @@
       <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>89</v>
+      <c r="C9" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -928,8 +935,8 @@
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>89</v>
+      <c r="C10" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -940,8 +947,8 @@
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>89</v>
+      <c r="C11" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -952,8 +959,8 @@
       <c r="B12" s="3">
         <v>7</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>89</v>
+      <c r="C12" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -964,8 +971,8 @@
       <c r="B13" s="3">
         <v>7</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>89</v>
+      <c r="C13" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -976,8 +983,8 @@
       <c r="B14" s="3">
         <v>7</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>89</v>
+      <c r="C14" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -988,8 +995,8 @@
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>89</v>
+      <c r="C15" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1000,8 +1007,8 @@
       <c r="B16" s="3">
         <v>7</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>90</v>
+      <c r="C16" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1012,8 +1019,8 @@
       <c r="B17" s="3">
         <v>7</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>90</v>
+      <c r="C17" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1024,20 +1031,20 @@
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>91</v>
+      <c r="C18" s="13" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="16">
+      <c r="A19" s="11">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="11">
         <v>2</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>92</v>
+      <c r="C19" s="14" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1053,7 +1060,7 @@
       <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1100,25 +1107,25 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
         <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="L2" s="6">
         <v>30</v>
@@ -1127,31 +1134,31 @@
         <v>31</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="T2" s="6">
         <v>2</v>
       </c>
       <c r="U2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="W2" s="6">
         <v>17</v>
@@ -1167,54 +1174,54 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="18"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="Q3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="R3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="S3" s="18"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="S3" s="12"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="10" t="s">
+      <c r="V3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="W3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3" s="13"/>
+      <c r="X3" s="19"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1253,7 +1260,7 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="20"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1284,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="14"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1310,7 +1317,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="4"/>
@@ -1371,7 +1378,7 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="20"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1402,7 +1409,7 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="20"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1427,7 +1434,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="str">
         <f>IF(ISBLANK(D11),"",COUNTA($D$5:D11))</f>
@@ -1462,8 +1469,8 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1493,8 +1500,8 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1524,8 +1531,8 @@
       <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1553,10 +1560,10 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+        <v>91</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1584,10 +1591,10 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
+        <v>52</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1611,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" t="str">
         <f>IF(ISBLANK(D17),"",COUNTA($D$5:D17))</f>
@@ -1645,11 +1652,11 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1677,11 +1684,11 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1709,10 +1716,10 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1740,11 +1747,11 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1772,11 +1779,11 @@
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1804,11 +1811,11 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1836,11 +1843,11 @@
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1868,11 +1875,11 @@
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1900,11 +1907,11 @@
         <v>19</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1928,7 +1935,7 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" t="str">
         <f>IF(ISBLANK(D27),"",COUNTA($D$5:D27))</f>
@@ -1964,12 +1971,12 @@
         <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="14"/>
+      <c r="H28" s="9"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -1996,12 +2003,12 @@
         <v>21</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="14"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2028,12 +2035,12 @@
         <v>22</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="14"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -2060,12 +2067,12 @@
         <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="14"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -2092,12 +2099,12 @@
         <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="14"/>
+      <c r="H32" s="9"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2124,12 +2131,12 @@
         <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="14"/>
+      <c r="H33" s="9"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2152,7 +2159,7 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C34" t="str">
         <f>IF(ISBLANK(D34),"",COUNTA($D$5:D34))</f>
@@ -2188,10 +2195,10 @@
         <v>26</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="14"/>
+      <c r="I35" s="9"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -2217,10 +2224,10 @@
         <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="14"/>
+      <c r="I36" s="9"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -2246,10 +2253,10 @@
         <v>28</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="14"/>
+      <c r="I37" s="9"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -2275,10 +2282,10 @@
         <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="14"/>
+      <c r="I38" s="9"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -2304,10 +2311,10 @@
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="14"/>
+      <c r="I39" s="9"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -2333,10 +2340,10 @@
         <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="14"/>
+      <c r="I40" s="9"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2358,7 +2365,7 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C41" t="str">
         <f>IF(ISBLANK(D41),"",COUNTA($D$5:D41))</f>
@@ -2394,10 +2401,10 @@
         <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="14"/>
+      <c r="I42" s="9"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2423,10 +2430,10 @@
         <v>33</v>
       </c>
       <c r="D43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="14"/>
+      <c r="I43" s="9"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2452,10 +2459,10 @@
         <v>34</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="14"/>
+      <c r="I44" s="9"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2481,10 +2488,10 @@
         <v>35</v>
       </c>
       <c r="D45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="14"/>
+      <c r="I45" s="9"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -2510,10 +2517,10 @@
         <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H46" s="1"/>
-      <c r="I46" s="14"/>
+      <c r="I46" s="9"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2539,10 +2546,10 @@
         <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="14"/>
+      <c r="I47" s="9"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -2564,7 +2571,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" t="str">
         <f>IF(ISBLANK(D48),"",COUNTA($D$5:D48))</f>
@@ -2600,11 +2607,11 @@
         <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="14"/>
+      <c r="J49" s="9"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -2629,11 +2636,11 @@
         <v>39</v>
       </c>
       <c r="D50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="14"/>
+      <c r="J50" s="9"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -2658,11 +2665,11 @@
         <v>40</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="14"/>
+      <c r="J51" s="9"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -2687,11 +2694,11 @@
         <v>41</v>
       </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="14"/>
+      <c r="J52" s="9"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
@@ -2716,11 +2723,11 @@
         <v>42</v>
       </c>
       <c r="D53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-      <c r="J53" s="14"/>
+      <c r="J53" s="9"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -2745,11 +2752,11 @@
         <v>43</v>
       </c>
       <c r="D54" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-      <c r="J54" s="14"/>
+      <c r="J54" s="9"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -2770,7 +2777,7 @@
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C55" t="str">
         <f>IF(ISBLANK(D55),"",COUNTA($D$5:D55))</f>
@@ -2806,12 +2813,12 @@
         <v>44</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="14"/>
+      <c r="K56" s="9"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
@@ -2835,12 +2842,12 @@
         <v>45</v>
       </c>
       <c r="D57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="14"/>
+      <c r="K57" s="9"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
@@ -2864,12 +2871,12 @@
         <v>46</v>
       </c>
       <c r="D58" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="14"/>
+      <c r="K58" s="9"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
@@ -2893,12 +2900,12 @@
         <v>47</v>
       </c>
       <c r="D59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="14"/>
+      <c r="K59" s="9"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
@@ -2922,12 +2929,12 @@
         <v>48</v>
       </c>
       <c r="D60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="14"/>
+      <c r="K60" s="9"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
@@ -2951,12 +2958,12 @@
         <v>49</v>
       </c>
       <c r="D61" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="14"/>
+      <c r="K61" s="9"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
@@ -2980,12 +2987,12 @@
         <v>50</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="14"/>
+      <c r="K62" s="9"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
@@ -3009,12 +3016,12 @@
         <v>51</v>
       </c>
       <c r="D63" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
-      <c r="K63" s="14"/>
+      <c r="K63" s="9"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
@@ -3034,7 +3041,7 @@
         <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C64" t="str">
         <f>IF(ISBLANK(D64),"",COUNTA($D$5:D64))</f>
@@ -3070,15 +3077,15 @@
         <v>52</v>
       </c>
       <c r="D65" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
-      <c r="L65" s="14"/>
-      <c r="M65" s="14"/>
-      <c r="N65" s="14"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
@@ -3099,15 +3106,15 @@
         <v>53</v>
       </c>
       <c r="D66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
@@ -3128,15 +3135,15 @@
         <v>54</v>
       </c>
       <c r="D67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -3157,15 +3164,15 @@
         <v>55</v>
       </c>
       <c r="D68" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
@@ -3186,15 +3193,15 @@
         <v>56</v>
       </c>
       <c r="D69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
-      <c r="L69" s="14"/>
-      <c r="M69" s="14"/>
-      <c r="N69" s="14"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
@@ -3215,15 +3222,15 @@
         <v>57</v>
       </c>
       <c r="D70" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="14"/>
-      <c r="N70" s="14"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
@@ -3240,7 +3247,7 @@
         <v>11</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C71" t="str">
         <f>IF(ISBLANK(D71),"",COUNTA($D$5:D71))</f>
@@ -3276,15 +3283,15 @@
         <v>58</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
@@ -3305,15 +3312,15 @@
         <v>59</v>
       </c>
       <c r="D73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
@@ -3334,15 +3341,15 @@
         <v>60</v>
       </c>
       <c r="D74" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
-      <c r="L74" s="14"/>
-      <c r="M74" s="14"/>
-      <c r="N74" s="14"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
       <c r="O74" s="1"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
@@ -3363,15 +3370,15 @@
         <v>61</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
-      <c r="L75" s="14"/>
-      <c r="M75" s="14"/>
-      <c r="N75" s="14"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
       <c r="O75" s="1"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
@@ -3392,15 +3399,15 @@
         <v>62</v>
       </c>
       <c r="D76" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
-      <c r="L76" s="14"/>
-      <c r="M76" s="14"/>
-      <c r="N76" s="14"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
       <c r="O76" s="1"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
@@ -3421,15 +3428,15 @@
         <v>63</v>
       </c>
       <c r="D77" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
-      <c r="L77" s="14"/>
-      <c r="M77" s="14"/>
-      <c r="N77" s="14"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
       <c r="O77" s="1"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
@@ -3450,15 +3457,15 @@
         <v>64</v>
       </c>
       <c r="D78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
-      <c r="L78" s="14"/>
-      <c r="M78" s="14"/>
-      <c r="N78" s="14"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
       <c r="O78" s="1"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
@@ -3475,7 +3482,7 @@
         <v>12</v>
       </c>
       <c r="B79" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C79" t="str">
         <f>IF(ISBLANK(D79),"",COUNTA($D$5:D79))</f>
@@ -3511,7 +3518,7 @@
         <v>65</v>
       </c>
       <c r="D80" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
@@ -3520,7 +3527,7 @@
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
-      <c r="O80" s="14"/>
+      <c r="O80" s="9"/>
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
@@ -3540,7 +3547,7 @@
         <v>66</v>
       </c>
       <c r="D81" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
@@ -3549,7 +3556,7 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
-      <c r="O81" s="14"/>
+      <c r="O81" s="9"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
@@ -3569,7 +3576,7 @@
         <v>67</v>
       </c>
       <c r="D82" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
@@ -3578,7 +3585,7 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
-      <c r="O82" s="14"/>
+      <c r="O82" s="9"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
@@ -3598,7 +3605,7 @@
         <v>68</v>
       </c>
       <c r="D83" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
@@ -3607,7 +3614,7 @@
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
-      <c r="O83" s="14"/>
+      <c r="O83" s="9"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
@@ -3627,7 +3634,7 @@
         <v>69</v>
       </c>
       <c r="D84" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -3636,7 +3643,7 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
-      <c r="O84" s="14"/>
+      <c r="O84" s="9"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
@@ -3656,7 +3663,7 @@
         <v>70</v>
       </c>
       <c r="D85" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
@@ -3665,7 +3672,7 @@
       <c r="L85" s="1"/>
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
-      <c r="O85" s="14"/>
+      <c r="O85" s="9"/>
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
       <c r="R85" s="1"/>
@@ -3681,7 +3688,7 @@
         <v>13</v>
       </c>
       <c r="B86" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C86" t="str">
         <f>IF(ISBLANK(D86),"",COUNTA($D$5:D86))</f>
@@ -3717,7 +3724,7 @@
         <v>71</v>
       </c>
       <c r="D87" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -3727,7 +3734,7 @@
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
-      <c r="P87" s="14"/>
+      <c r="P87" s="9"/>
       <c r="Q87" s="1"/>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
@@ -3746,7 +3753,7 @@
         <v>72</v>
       </c>
       <c r="D88" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -3756,7 +3763,7 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
-      <c r="P88" s="14"/>
+      <c r="P88" s="9"/>
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
@@ -3775,7 +3782,7 @@
         <v>73</v>
       </c>
       <c r="D89" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -3785,7 +3792,7 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
-      <c r="P89" s="14"/>
+      <c r="P89" s="9"/>
       <c r="Q89" s="1"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
@@ -3804,7 +3811,7 @@
         <v>74</v>
       </c>
       <c r="D90" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -3814,7 +3821,7 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
-      <c r="P90" s="14"/>
+      <c r="P90" s="9"/>
       <c r="Q90" s="1"/>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
@@ -3833,7 +3840,7 @@
         <v>75</v>
       </c>
       <c r="D91" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -3843,7 +3850,7 @@
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
-      <c r="P91" s="14"/>
+      <c r="P91" s="9"/>
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
@@ -3862,7 +3869,7 @@
         <v>76</v>
       </c>
       <c r="D92" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -3872,7 +3879,7 @@
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
-      <c r="P92" s="14"/>
+      <c r="P92" s="9"/>
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
       <c r="S92" s="1"/>
@@ -3887,7 +3894,7 @@
         <v>14</v>
       </c>
       <c r="B93" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C93" t="str">
         <f>IF(ISBLANK(D93),"",COUNTA($D$5:D93))</f>
@@ -3920,10 +3927,10 @@
         <v>77</v>
       </c>
       <c r="D94" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H94" s="1"/>
-      <c r="I94" s="14"/>
+      <c r="I94" s="9"/>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
@@ -3949,7 +3956,7 @@
         <v>78</v>
       </c>
       <c r="D95" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
@@ -3960,7 +3967,7 @@
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
-      <c r="Q95" s="14"/>
+      <c r="Q95" s="9"/>
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
@@ -3974,7 +3981,7 @@
         <v>15</v>
       </c>
       <c r="B96" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C96" t="str">
         <f>IF(ISBLANK(D96),"",COUNTA($D$5:D96))</f>
@@ -4007,7 +4014,7 @@
         <v>79</v>
       </c>
       <c r="D97" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
@@ -4018,7 +4025,7 @@
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
-      <c r="Q97" s="14"/>
+      <c r="Q97" s="9"/>
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
@@ -4036,7 +4043,7 @@
         <v>80</v>
       </c>
       <c r="D98" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
@@ -4047,7 +4054,7 @@
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
-      <c r="Q98" s="14"/>
+      <c r="Q98" s="9"/>
       <c r="R98" s="1"/>
       <c r="S98" s="1"/>
       <c r="T98" s="1"/>
@@ -4061,7 +4068,7 @@
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C99" t="str">
         <f>IF(ISBLANK(D99),"",COUNTA($D$5:D99))</f>
@@ -4094,7 +4101,7 @@
         <v>81</v>
       </c>
       <c r="D100" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
@@ -4106,9 +4113,9 @@
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
-      <c r="R100" s="14"/>
-      <c r="S100" s="14"/>
-      <c r="T100" s="14"/>
+      <c r="R100" s="9"/>
+      <c r="S100" s="9"/>
+      <c r="T100" s="9"/>
       <c r="U100" s="1"/>
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
@@ -4123,7 +4130,7 @@
         <v>82</v>
       </c>
       <c r="D101" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
@@ -4135,9 +4142,9 @@
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
-      <c r="R101" s="14"/>
-      <c r="S101" s="14"/>
-      <c r="T101" s="14"/>
+      <c r="R101" s="9"/>
+      <c r="S101" s="9"/>
+      <c r="T101" s="9"/>
       <c r="U101" s="1"/>
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
@@ -4196,9 +4203,9 @@
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
       <c r="T103" s="1"/>
-      <c r="U103" s="14"/>
-      <c r="V103" s="14"/>
-      <c r="W103" s="14"/>
+      <c r="U103" s="9"/>
+      <c r="V103" s="9"/>
+      <c r="W103" s="9"/>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A104" t="str">
@@ -4225,9 +4232,9 @@
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
       <c r="T104" s="1"/>
-      <c r="U104" s="14"/>
-      <c r="V104" s="14"/>
-      <c r="W104" s="14"/>
+      <c r="U104" s="9"/>
+      <c r="V104" s="9"/>
+      <c r="W104" s="9"/>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A105" t="str">
@@ -4239,27 +4246,27 @@
         <v>85</v>
       </c>
       <c r="D105" t="s">
-        <v>87</v>
-      </c>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-      <c r="G105" s="14"/>
-      <c r="H105" s="14"/>
-      <c r="I105" s="14"/>
-      <c r="J105" s="14"/>
-      <c r="K105" s="14"/>
-      <c r="L105" s="14"/>
-      <c r="M105" s="14"/>
-      <c r="N105" s="14"/>
-      <c r="O105" s="14"/>
-      <c r="P105" s="14"/>
-      <c r="Q105" s="14"/>
-      <c r="R105" s="14"/>
-      <c r="S105" s="14"/>
-      <c r="T105" s="14"/>
-      <c r="U105" s="14"/>
-      <c r="V105" s="14"/>
-      <c r="W105" s="14"/>
+        <v>85</v>
+      </c>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="9"/>
+      <c r="M105" s="9"/>
+      <c r="N105" s="9"/>
+      <c r="O105" s="9"/>
+      <c r="P105" s="9"/>
+      <c r="Q105" s="9"/>
+      <c r="R105" s="9"/>
+      <c r="S105" s="9"/>
+      <c r="T105" s="9"/>
+      <c r="U105" s="9"/>
+      <c r="V105" s="9"/>
+      <c r="W105" s="9"/>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A106">

</xml_diff>

<commit_message>
Added privacy policy and terms and conditions
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B25A623-B81A-485D-9F37-4EA9B6B85836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649EED77-9C67-4988-981F-4FA4A2F1192B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="93">
   <si>
     <t>June</t>
   </si>
@@ -482,6 +482,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -497,7 +498,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,7 +1060,7 @@
       <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1177,10 +1177,10 @@
       <c r="E3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="16"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
@@ -1193,11 +1193,11 @@
       <c r="K3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="17" t="s">
+      <c r="L3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20"/>
       <c r="O3" s="8" t="s">
         <v>45</v>
       </c>
@@ -1207,21 +1207,21 @@
       <c r="Q3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="R3" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="18"/>
-      <c r="T3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="20"/>
       <c r="U3" s="8" t="s">
         <v>49</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="W3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="19"/>
+      <c r="X3" s="20"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1260,7 +1260,7 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="15"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1378,7 +1378,7 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="20"/>
+      <c r="E9" s="15"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1409,7 +1409,7 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="15"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1469,8 +1469,8 @@
       <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1500,8 +1500,8 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1531,8 +1531,8 @@
       <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1562,8 +1562,8 @@
       <c r="D15" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1593,8 +1593,8 @@
       <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>

</xml_diff>

<commit_message>
working form submission to create new trip
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFE670C-AC3D-47A7-94E2-86BA6A4D7D29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D8EE6-A2CA-49EB-8131-BBDBD3AD673B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -486,6 +486,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -501,7 +502,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,10 +1061,10 @@
   <dimension ref="A1:X107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="23" ySplit="3" topLeftCell="X10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1181,10 +1181,10 @@
       <c r="E3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
@@ -1197,11 +1197,11 @@
       <c r="K3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="8" t="s">
         <v>45</v>
       </c>
@@ -1211,21 +1211,21 @@
       <c r="Q3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="19"/>
-      <c r="T3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="8" t="s">
         <v>49</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="W3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="20"/>
+      <c r="X3" s="21"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1786,8 +1786,8 @@
         <v>56</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1948,7 +1948,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="9"/>
+      <c r="H27" s="15"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1980,7 +1980,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="9"/>
+      <c r="H28" s="15"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2012,7 +2012,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="15"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2076,7 +2076,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="15"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>

</xml_diff>

<commit_message>
Implemented Update, Delete DB operations and made trips page fully integrated with DB actions vs previous mock objects
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D8EE6-A2CA-49EB-8131-BBDBD3AD673B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA0418C-1A66-47C4-B489-B5A20E244D42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="92">
   <si>
     <t>June</t>
   </si>
@@ -319,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,12 +341,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -486,7 +480,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1064,7 +1057,7 @@
       <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1181,10 +1174,10 @@
       <c r="E3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="17"/>
       <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
@@ -1197,11 +1190,11 @@
       <c r="K3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="20"/>
       <c r="O3" s="8" t="s">
         <v>45</v>
       </c>
@@ -1211,21 +1204,21 @@
       <c r="Q3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="R3" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="20"/>
-      <c r="T3" s="21"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="20"/>
       <c r="U3" s="8" t="s">
         <v>49</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="W3" s="19" t="s">
+      <c r="W3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="21"/>
+      <c r="X3" s="20"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1754,8 +1747,8 @@
         <v>55</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1786,8 +1779,8 @@
         <v>56</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2044,7 +2037,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="9"/>
+      <c r="H30" s="15"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>

</xml_diff>

<commit_message>
Added settings router - get current user notifications settings
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA0418C-1A66-47C4-B489-B5A20E244D42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45FE7F6-AAF9-4F5D-8F75-9860274D4690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
   <si>
     <t>June</t>
   </si>
@@ -207,9 +207,6 @@
   </si>
   <si>
     <t>new trip page</t>
-  </si>
-  <si>
-    <t>contact us page</t>
   </si>
   <si>
     <t>settings page</t>
@@ -319,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -495,6 +498,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,7 +828,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -873,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -885,7 +889,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -897,7 +901,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -909,7 +913,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -921,7 +925,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -933,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -945,7 +949,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -957,7 +961,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -969,7 +973,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -981,7 +985,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -993,7 +997,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1005,7 +1009,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -1017,7 +1021,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1029,7 +1033,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1041,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1051,13 +1055,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88B0EE7-956E-4B03-A664-44669239B7CE}">
-  <dimension ref="A1:X107"/>
+  <dimension ref="A1:X100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1314,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="4"/>
@@ -1557,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1652,17 +1656,17 @@
         <v>53</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1684,17 +1688,17 @@
         <v>54</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -1808,11 +1812,11 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1840,7 +1844,7 @@
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="15"/>
@@ -1872,7 +1876,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="9"/>
@@ -1936,7 +1940,7 @@
         <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2096,12 +2100,12 @@
         <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="9"/>
+      <c r="H32" s="15"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2160,10 +2164,10 @@
         <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="9"/>
+      <c r="I34" s="15"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -2192,7 +2196,7 @@
         <v>54</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="9"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -2279,7 +2283,7 @@
         <v>56</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="9"/>
+      <c r="I38" s="15"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -2305,7 +2309,7 @@
         <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="9"/>
@@ -2366,11 +2370,11 @@
         <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="9"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2398,8 +2402,8 @@
         <v>54</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="9"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2427,8 +2431,8 @@
         <v>57</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="9"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -2456,8 +2460,8 @@
         <v>55</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="9"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -2485,8 +2489,8 @@
         <v>56</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="9"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -2511,11 +2515,11 @@
         <v>36</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H46" s="1"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="9"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -2572,12 +2576,12 @@
         <v>37</v>
       </c>
       <c r="D48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="9"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
@@ -2605,8 +2609,8 @@
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="9"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
@@ -2634,8 +2638,8 @@
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="9"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
@@ -2663,8 +2667,8 @@
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="9"/>
-      <c r="K51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="9"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
@@ -2692,8 +2696,8 @@
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="9"/>
-      <c r="K52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="9"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
@@ -2717,12 +2721,12 @@
         <v>42</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-      <c r="J53" s="9"/>
-      <c r="K53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="9"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
@@ -2736,25 +2740,22 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A54">
+    <row r="54" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+      <c r="A54" t="str">
         <f>IF(ISBLANK(B54),"",COUNTA($B$4:B54))</f>
-        <v>9</v>
-      </c>
-      <c r="B54" t="s">
-        <v>63</v>
-      </c>
-      <c r="C54" t="str">
+        <v/>
+      </c>
+      <c r="C54">
         <f>IF(ISBLANK(D54),"",COUNTA($D$5:D54))</f>
-        <v/>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
+      <c r="K54" s="9"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
@@ -2775,10 +2776,10 @@
       </c>
       <c r="C55">
         <f>IF(ISBLANK(D55),"",COUNTA($D$5:D55))</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D55" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
@@ -2798,21 +2799,24 @@
       <c r="W55" s="1"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A56" t="str">
+      <c r="A56">
         <f>IF(ISBLANK(B56),"",COUNTA($B$4:B56))</f>
-        <v/>
-      </c>
-      <c r="C56">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" t="str">
         <f>IF(ISBLANK(D56),"",COUNTA($D$5:D56))</f>
-        <v>44</v>
-      </c>
-      <c r="D56" t="s">
-        <v>54</v>
-      </c>
+        <v/>
+      </c>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
-      <c r="K56" s="9"/>
+      <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
@@ -2836,15 +2840,15 @@
         <v>45</v>
       </c>
       <c r="D57" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
@@ -2865,15 +2869,15 @@
         <v>46</v>
       </c>
       <c r="D58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
-      <c r="K58" s="9"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
@@ -2894,15 +2898,15 @@
         <v>47</v>
       </c>
       <c r="D59" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
-      <c r="K59" s="9"/>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
@@ -2923,15 +2927,15 @@
         <v>48</v>
       </c>
       <c r="D60" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
-      <c r="K60" s="9"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
@@ -2942,7 +2946,7 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
     </row>
-    <row r="61" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f>IF(ISBLANK(B61),"",COUNTA($B$4:B61))</f>
         <v/>
@@ -2951,16 +2955,16 @@
         <f>IF(ISBLANK(D61),"",COUNTA($D$5:D61))</f>
         <v>49</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>80</v>
+      <c r="D61" t="s">
+        <v>56</v>
       </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
-      <c r="K61" s="9"/>
-      <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
@@ -2981,15 +2985,15 @@
         <v>50</v>
       </c>
       <c r="D62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
@@ -3042,7 +3046,7 @@
         <v>51</v>
       </c>
       <c r="D64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -3187,7 +3191,7 @@
         <v>56</v>
       </c>
       <c r="D69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
@@ -3207,27 +3211,24 @@
       <c r="W69" s="1"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A70">
+      <c r="A70" t="str">
         <f>IF(ISBLANK(B70),"",COUNTA($B$4:B70))</f>
-        <v>11</v>
-      </c>
-      <c r="B70" t="s">
-        <v>65</v>
-      </c>
-      <c r="C70" t="str">
+        <v/>
+      </c>
+      <c r="C70">
         <f>IF(ISBLANK(D70),"",COUNTA($D$5:D70))</f>
-        <v/>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="D70" t="s">
+        <v>68</v>
+      </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
@@ -3239,24 +3240,27 @@
       <c r="W70" s="1"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A71" t="str">
+      <c r="A71">
         <f>IF(ISBLANK(B71),"",COUNTA($B$4:B71))</f>
-        <v/>
-      </c>
-      <c r="C71">
+        <v>11</v>
+      </c>
+      <c r="B71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" t="str">
         <f>IF(ISBLANK(D71),"",COUNTA($D$5:D71))</f>
-        <v>57</v>
-      </c>
-      <c r="D71" t="s">
-        <v>70</v>
-      </c>
+        <v/>
+      </c>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
-      <c r="L71" s="9"/>
-      <c r="M71" s="9"/>
-      <c r="N71" s="9"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
       <c r="O71" s="1"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
@@ -3277,16 +3281,16 @@
         <v>58</v>
       </c>
       <c r="D72" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
-      <c r="L72" s="9"/>
-      <c r="M72" s="9"/>
-      <c r="N72" s="9"/>
-      <c r="O72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="9"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -3306,16 +3310,16 @@
         <v>59</v>
       </c>
       <c r="D73" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
-      <c r="L73" s="9"/>
-      <c r="M73" s="9"/>
-      <c r="N73" s="9"/>
-      <c r="O73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="9"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
@@ -3335,16 +3339,16 @@
         <v>60</v>
       </c>
       <c r="D74" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
-      <c r="N74" s="9"/>
-      <c r="O74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="9"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
@@ -3364,16 +3368,16 @@
         <v>61</v>
       </c>
       <c r="D75" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
-      <c r="N75" s="9"/>
-      <c r="O75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="9"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
@@ -3393,16 +3397,16 @@
         <v>62</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
-      <c r="N76" s="9"/>
-      <c r="O76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="9"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
@@ -3422,16 +3426,16 @@
         <v>63</v>
       </c>
       <c r="D77" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="9"/>
-      <c r="O77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="9"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
@@ -3483,7 +3487,7 @@
         <v>64</v>
       </c>
       <c r="D79" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
@@ -3492,8 +3496,8 @@
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
-      <c r="O79" s="9"/>
-      <c r="P79" s="1"/>
+      <c r="O79" s="1"/>
+      <c r="P79" s="9"/>
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
@@ -3521,8 +3525,8 @@
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
-      <c r="O80" s="9"/>
-      <c r="P80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="9"/>
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
@@ -3550,8 +3554,8 @@
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
-      <c r="O81" s="9"/>
-      <c r="P81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="9"/>
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
@@ -3579,8 +3583,8 @@
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
-      <c r="O82" s="9"/>
-      <c r="P82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="9"/>
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
@@ -3608,8 +3612,8 @@
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
-      <c r="O83" s="9"/>
-      <c r="P83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="9"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
@@ -3628,7 +3632,7 @@
         <v>69</v>
       </c>
       <c r="D84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
@@ -3637,8 +3641,8 @@
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
-      <c r="O84" s="9"/>
-      <c r="P84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="9"/>
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>
@@ -3653,15 +3657,12 @@
         <v>13</v>
       </c>
       <c r="B85" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C85" t="str">
         <f>IF(ISBLANK(D85),"",COUNTA($D$5:D85))</f>
         <v/>
       </c>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
@@ -3689,17 +3690,17 @@
         <v>70</v>
       </c>
       <c r="D86" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
+      <c r="I86" s="15"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
-      <c r="P86" s="9"/>
+      <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
@@ -3718,7 +3719,7 @@
         <v>71</v>
       </c>
       <c r="D87" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
@@ -3728,8 +3729,8 @@
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
-      <c r="P87" s="9"/>
-      <c r="Q87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="9"/>
       <c r="R87" s="1"/>
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
@@ -3738,16 +3739,16 @@
       <c r="W87" s="1"/>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A88" t="str">
+      <c r="A88">
         <f>IF(ISBLANK(B88),"",COUNTA($B$4:B88))</f>
-        <v/>
-      </c>
-      <c r="C88">
+        <v>14</v>
+      </c>
+      <c r="B88" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" t="str">
         <f>IF(ISBLANK(D88),"",COUNTA($D$5:D88))</f>
-        <v>72</v>
-      </c>
-      <c r="D88" t="s">
-        <v>57</v>
+        <v/>
       </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
@@ -3757,7 +3758,7 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
-      <c r="P88" s="9"/>
+      <c r="P88" s="1"/>
       <c r="Q88" s="1"/>
       <c r="R88" s="1"/>
       <c r="S88" s="1"/>
@@ -3773,10 +3774,10 @@
       </c>
       <c r="C89">
         <f>IF(ISBLANK(D89),"",COUNTA($D$5:D89))</f>
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D89" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
@@ -3786,8 +3787,8 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
-      <c r="P89" s="9"/>
-      <c r="Q89" s="1"/>
+      <c r="P89" s="1"/>
+      <c r="Q89" s="9"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
@@ -3802,10 +3803,10 @@
       </c>
       <c r="C90">
         <f>IF(ISBLANK(D90),"",COUNTA($D$5:D90))</f>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D90" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
@@ -3815,8 +3816,8 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
-      <c r="P90" s="9"/>
-      <c r="Q90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="9"/>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
@@ -3825,16 +3826,16 @@
       <c r="W90" s="1"/>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A91" t="str">
+      <c r="A91">
         <f>IF(ISBLANK(B91),"",COUNTA($B$4:B91))</f>
-        <v/>
-      </c>
-      <c r="C91">
+        <v>15</v>
+      </c>
+      <c r="B91" t="s">
+        <v>73</v>
+      </c>
+      <c r="C91" t="str">
         <f>IF(ISBLANK(D91),"",COUNTA($D$5:D91))</f>
-        <v>75</v>
-      </c>
-      <c r="D91" t="s">
-        <v>91</v>
+        <v/>
       </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
@@ -3844,7 +3845,7 @@
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
-      <c r="P91" s="9"/>
+      <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
@@ -3854,16 +3855,16 @@
       <c r="W91" s="1"/>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A92">
+      <c r="A92" t="str">
         <f>IF(ISBLANK(B92),"",COUNTA($B$4:B92))</f>
-        <v>14</v>
-      </c>
-      <c r="B92" t="s">
-        <v>71</v>
-      </c>
-      <c r="C92" t="str">
+        <v/>
+      </c>
+      <c r="C92">
         <f>IF(ISBLANK(D92),"",COUNTA($D$5:D92))</f>
-        <v/>
+        <v>74</v>
+      </c>
+      <c r="D92" t="s">
+        <v>74</v>
       </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
@@ -3875,9 +3876,9 @@
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
-      <c r="R92" s="1"/>
-      <c r="S92" s="1"/>
-      <c r="T92" s="1"/>
+      <c r="R92" s="9"/>
+      <c r="S92" s="9"/>
+      <c r="T92" s="9"/>
       <c r="U92" s="1"/>
       <c r="V92" s="1"/>
       <c r="W92" s="1"/>
@@ -3889,13 +3890,13 @@
       </c>
       <c r="C93">
         <f>IF(ISBLANK(D93),"",COUNTA($D$5:D93))</f>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D93" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H93" s="1"/>
-      <c r="I93" s="15"/>
+      <c r="I93" s="1"/>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
@@ -3904,24 +3905,24 @@
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
-      <c r="R93" s="1"/>
-      <c r="S93" s="1"/>
-      <c r="T93" s="1"/>
+      <c r="R93" s="9"/>
+      <c r="S93" s="9"/>
+      <c r="T93" s="9"/>
       <c r="U93" s="1"/>
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A94" t="str">
+      <c r="A94">
         <f>IF(ISBLANK(B94),"",COUNTA($B$4:B94))</f>
-        <v/>
-      </c>
-      <c r="C94">
+        <v>16</v>
+      </c>
+      <c r="B94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C94" t="str">
         <f>IF(ISBLANK(D94),"",COUNTA($D$5:D94))</f>
-        <v>77</v>
-      </c>
-      <c r="D94" t="s">
-        <v>73</v>
+        <v/>
       </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
@@ -3932,7 +3933,7 @@
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
       <c r="P94" s="1"/>
-      <c r="Q94" s="9"/>
+      <c r="Q94" s="1"/>
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
@@ -3941,16 +3942,16 @@
       <c r="W94" s="1"/>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A95">
+      <c r="A95" t="str">
         <f>IF(ISBLANK(B95),"",COUNTA($B$4:B95))</f>
-        <v>15</v>
-      </c>
-      <c r="B95" t="s">
-        <v>77</v>
-      </c>
-      <c r="C95" t="str">
+        <v/>
+      </c>
+      <c r="C95">
         <f>IF(ISBLANK(D95),"",COUNTA($D$5:D95))</f>
-        <v/>
+        <v>76</v>
+      </c>
+      <c r="D95" t="s">
+        <v>5</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
@@ -3965,9 +3966,9 @@
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
-      <c r="U95" s="1"/>
-      <c r="V95" s="1"/>
-      <c r="W95" s="1"/>
+      <c r="U95" s="9"/>
+      <c r="V95" s="9"/>
+      <c r="W95" s="9"/>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A96" t="str">
@@ -3976,10 +3977,10 @@
       </c>
       <c r="C96">
         <f>IF(ISBLANK(D96),"",COUNTA($D$5:D96))</f>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D96" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
@@ -3990,13 +3991,13 @@
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
-      <c r="Q96" s="9"/>
+      <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
-      <c r="U96" s="1"/>
-      <c r="V96" s="1"/>
-      <c r="W96" s="1"/>
+      <c r="U96" s="9"/>
+      <c r="V96" s="9"/>
+      <c r="W96" s="9"/>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A97" t="str">
@@ -4005,35 +4006,38 @@
       </c>
       <c r="C97">
         <f>IF(ISBLANK(D97),"",COUNTA($D$5:D97))</f>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D97" t="s">
-        <v>79</v>
-      </c>
-      <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-      <c r="K97" s="1"/>
-      <c r="L97" s="1"/>
-      <c r="M97" s="1"/>
-      <c r="N97" s="1"/>
-      <c r="O97" s="1"/>
-      <c r="P97" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="9"/>
+      <c r="K97" s="9"/>
+      <c r="L97" s="9"/>
+      <c r="M97" s="9"/>
+      <c r="N97" s="9"/>
+      <c r="O97" s="9"/>
+      <c r="P97" s="9"/>
       <c r="Q97" s="9"/>
-      <c r="R97" s="1"/>
-      <c r="S97" s="1"/>
-      <c r="T97" s="1"/>
-      <c r="U97" s="1"/>
-      <c r="V97" s="1"/>
-      <c r="W97" s="1"/>
+      <c r="R97" s="9"/>
+      <c r="S97" s="9"/>
+      <c r="T97" s="9"/>
+      <c r="U97" s="9"/>
+      <c r="V97" s="9"/>
+      <c r="W97" s="9"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A98">
         <f>IF(ISBLANK(B98),"",COUNTA($B$4:B98))</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="C98" t="str">
         <f>IF(ISBLANK(D98),"",COUNTA($D$5:D98))</f>
@@ -4055,19 +4059,9 @@
       <c r="U98" s="1"/>
       <c r="V98" s="1"/>
       <c r="W98" s="1"/>
+      <c r="X98" s="4"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A99" t="str">
-        <f>IF(ISBLANK(B99),"",COUNTA($B$4:B99))</f>
-        <v/>
-      </c>
-      <c r="C99">
-        <f>IF(ISBLANK(D99),"",COUNTA($D$5:D99))</f>
-        <v>80</v>
-      </c>
-      <c r="D99" t="s">
-        <v>75</v>
-      </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
@@ -4078,25 +4072,14 @@
       <c r="O99" s="1"/>
       <c r="P99" s="1"/>
       <c r="Q99" s="1"/>
-      <c r="R99" s="9"/>
-      <c r="S99" s="9"/>
-      <c r="T99" s="9"/>
+      <c r="R99" s="1"/>
+      <c r="S99" s="1"/>
+      <c r="T99" s="1"/>
       <c r="U99" s="1"/>
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A100" t="str">
-        <f>IF(ISBLANK(B100),"",COUNTA($B$4:B100))</f>
-        <v/>
-      </c>
-      <c r="C100">
-        <f>IF(ISBLANK(D100),"",COUNTA($D$5:D100))</f>
-        <v>81</v>
-      </c>
-      <c r="D100" t="s">
-        <v>76</v>
-      </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
@@ -4107,197 +4090,12 @@
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
-      <c r="R100" s="9"/>
-      <c r="S100" s="9"/>
-      <c r="T100" s="9"/>
+      <c r="R100" s="1"/>
+      <c r="S100" s="1"/>
+      <c r="T100" s="1"/>
       <c r="U100" s="1"/>
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A101">
-        <f>IF(ISBLANK(B101),"",COUNTA($B$4:B101))</f>
-        <v>17</v>
-      </c>
-      <c r="B101" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101" t="str">
-        <f>IF(ISBLANK(D101),"",COUNTA($D$5:D101))</f>
-        <v/>
-      </c>
-      <c r="H101" s="1"/>
-      <c r="I101" s="1"/>
-      <c r="J101" s="1"/>
-      <c r="K101" s="1"/>
-      <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
-      <c r="P101" s="1"/>
-      <c r="Q101" s="1"/>
-      <c r="R101" s="1"/>
-      <c r="S101" s="1"/>
-      <c r="T101" s="1"/>
-      <c r="U101" s="1"/>
-      <c r="V101" s="1"/>
-      <c r="W101" s="1"/>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A102" t="str">
-        <f>IF(ISBLANK(B102),"",COUNTA($B$4:B102))</f>
-        <v/>
-      </c>
-      <c r="C102">
-        <f>IF(ISBLANK(D102),"",COUNTA($D$5:D102))</f>
-        <v>82</v>
-      </c>
-      <c r="D102" t="s">
-        <v>5</v>
-      </c>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
-      <c r="O102" s="1"/>
-      <c r="P102" s="1"/>
-      <c r="Q102" s="1"/>
-      <c r="R102" s="1"/>
-      <c r="S102" s="1"/>
-      <c r="T102" s="1"/>
-      <c r="U102" s="9"/>
-      <c r="V102" s="9"/>
-      <c r="W102" s="9"/>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A103" t="str">
-        <f>IF(ISBLANK(B103),"",COUNTA($B$4:B103))</f>
-        <v/>
-      </c>
-      <c r="C103">
-        <f>IF(ISBLANK(D103),"",COUNTA($D$5:D103))</f>
-        <v>83</v>
-      </c>
-      <c r="D103" t="s">
-        <v>22</v>
-      </c>
-      <c r="H103" s="1"/>
-      <c r="I103" s="1"/>
-      <c r="J103" s="1"/>
-      <c r="K103" s="1"/>
-      <c r="L103" s="1"/>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
-      <c r="O103" s="1"/>
-      <c r="P103" s="1"/>
-      <c r="Q103" s="1"/>
-      <c r="R103" s="1"/>
-      <c r="S103" s="1"/>
-      <c r="T103" s="1"/>
-      <c r="U103" s="9"/>
-      <c r="V103" s="9"/>
-      <c r="W103" s="9"/>
-    </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A104" t="str">
-        <f>IF(ISBLANK(B104),"",COUNTA($B$4:B104))</f>
-        <v/>
-      </c>
-      <c r="C104">
-        <f>IF(ISBLANK(D104),"",COUNTA($D$5:D104))</f>
-        <v>84</v>
-      </c>
-      <c r="D104" t="s">
-        <v>84</v>
-      </c>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="9"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="9"/>
-      <c r="N104" s="9"/>
-      <c r="O104" s="9"/>
-      <c r="P104" s="9"/>
-      <c r="Q104" s="9"/>
-      <c r="R104" s="9"/>
-      <c r="S104" s="9"/>
-      <c r="T104" s="9"/>
-      <c r="U104" s="9"/>
-      <c r="V104" s="9"/>
-      <c r="W104" s="9"/>
-    </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A105">
-        <f>IF(ISBLANK(B105),"",COUNTA($B$4:B105))</f>
-        <v>18</v>
-      </c>
-      <c r="B105" t="s">
-        <v>6</v>
-      </c>
-      <c r="C105" t="str">
-        <f>IF(ISBLANK(D105),"",COUNTA($D$5:D105))</f>
-        <v/>
-      </c>
-      <c r="H105" s="1"/>
-      <c r="I105" s="1"/>
-      <c r="J105" s="1"/>
-      <c r="K105" s="1"/>
-      <c r="L105" s="1"/>
-      <c r="M105" s="1"/>
-      <c r="N105" s="1"/>
-      <c r="O105" s="1"/>
-      <c r="P105" s="1"/>
-      <c r="Q105" s="1"/>
-      <c r="R105" s="1"/>
-      <c r="S105" s="1"/>
-      <c r="T105" s="1"/>
-      <c r="U105" s="1"/>
-      <c r="V105" s="1"/>
-      <c r="W105" s="1"/>
-      <c r="X105" s="4"/>
-    </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="H106" s="1"/>
-      <c r="I106" s="1"/>
-      <c r="J106" s="1"/>
-      <c r="K106" s="1"/>
-      <c r="L106" s="1"/>
-      <c r="M106" s="1"/>
-      <c r="N106" s="1"/>
-      <c r="O106" s="1"/>
-      <c r="P106" s="1"/>
-      <c r="Q106" s="1"/>
-      <c r="R106" s="1"/>
-      <c r="S106" s="1"/>
-      <c r="T106" s="1"/>
-      <c r="U106" s="1"/>
-      <c r="V106" s="1"/>
-      <c r="W106" s="1"/>
-    </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="H107" s="1"/>
-      <c r="I107" s="1"/>
-      <c r="J107" s="1"/>
-      <c r="K107" s="1"/>
-      <c r="L107" s="1"/>
-      <c r="M107" s="1"/>
-      <c r="N107" s="1"/>
-      <c r="O107" s="1"/>
-      <c r="P107" s="1"/>
-      <c r="Q107" s="1"/>
-      <c r="R107" s="1"/>
-      <c r="S107" s="1"/>
-      <c r="T107" s="1"/>
-      <c r="U107" s="1"/>
-      <c r="V107" s="1"/>
-      <c r="W107" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Functioning toggles save settings preferences to DB
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45FE7F6-AAF9-4F5D-8F75-9860274D4690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA26B2A-3CA5-46D2-9424-1FF29B838FE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="91">
   <si>
     <t>June</t>
   </si>
@@ -483,6 +483,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,7 +499,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,7 +1061,7 @@
       <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1178,10 +1178,10 @@
       <c r="E3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
@@ -1194,11 +1194,11 @@
       <c r="K3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="19"/>
-      <c r="N3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="8" t="s">
         <v>45</v>
       </c>
@@ -1208,21 +1208,21 @@
       <c r="Q3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="19"/>
-      <c r="T3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="8" t="s">
         <v>49</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="W3" s="18" t="s">
+      <c r="W3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="20"/>
+      <c r="X3" s="21"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1656,17 +1656,17 @@
         <v>53</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1688,17 +1688,17 @@
         <v>54</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -2225,7 +2225,7 @@
         <v>57</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="9"/>
+      <c r="I36" s="15"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -2254,7 +2254,7 @@
         <v>55</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="9"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>

</xml_diff>

<commit_message>
Added needed beta test code to register
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA26B2A-3CA5-46D2-9424-1FF29B838FE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF8ABC8-DD06-4078-BBDE-A0A033727EE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="91">
   <si>
     <t>June</t>
   </si>
@@ -1061,7 +1061,7 @@
       <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1879,8 +1879,8 @@
         <v>80</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2312,7 +2312,7 @@
         <v>90</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="9"/>
+      <c r="I39" s="15"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>

</xml_diff>

<commit_message>
Fixed user creation in DB when using local emulator
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CC1C70-CE4A-45B5-A160-DF7895DB1EDF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624FA42F-BFE9-4FFF-9BF8-280A9A60CE30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="92">
   <si>
     <t>June</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t xml:space="preserve">unit tests </t>
+  </si>
+  <si>
+    <t>Submit draft final report</t>
   </si>
 </sst>
 </file>
@@ -1055,13 +1058,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B88B0EE7-956E-4B03-A664-44669239B7CE}">
-  <dimension ref="A1:X100"/>
+  <dimension ref="A1:X101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="3" topLeftCell="X40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3942,16 +3945,12 @@
       <c r="W94" s="1"/>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A95" t="str">
-        <f>IF(ISBLANK(B95),"",COUNTA($B$4:B95))</f>
-        <v/>
-      </c>
       <c r="C95">
         <f>IF(ISBLANK(D95),"",COUNTA($D$5:D95))</f>
         <v>76</v>
       </c>
       <c r="D95" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
@@ -3963,12 +3962,12 @@
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
-      <c r="R95" s="1"/>
+      <c r="R95" s="4"/>
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
-      <c r="U95" s="9"/>
-      <c r="V95" s="9"/>
-      <c r="W95" s="9"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A96" t="str">
@@ -3980,7 +3979,7 @@
         <v>77</v>
       </c>
       <c r="D96" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
@@ -4009,59 +4008,69 @@
         <v>78</v>
       </c>
       <c r="D97" t="s">
-        <v>83</v>
-      </c>
-      <c r="E97" s="9"/>
-      <c r="F97" s="9"/>
-      <c r="G97" s="9"/>
-      <c r="H97" s="9"/>
-      <c r="I97" s="9"/>
-      <c r="J97" s="9"/>
-      <c r="K97" s="9"/>
-      <c r="L97" s="9"/>
-      <c r="M97" s="9"/>
-      <c r="N97" s="9"/>
-      <c r="O97" s="9"/>
-      <c r="P97" s="9"/>
-      <c r="Q97" s="9"/>
-      <c r="R97" s="9"/>
-      <c r="S97" s="9"/>
-      <c r="T97" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+      <c r="R97" s="1"/>
+      <c r="S97" s="1"/>
+      <c r="T97" s="1"/>
       <c r="U97" s="9"/>
       <c r="V97" s="9"/>
       <c r="W97" s="9"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A98">
+      <c r="A98" t="str">
         <f>IF(ISBLANK(B98),"",COUNTA($B$4:B98))</f>
+        <v/>
+      </c>
+      <c r="C98">
+        <f>IF(ISBLANK(D98),"",COUNTA($D$5:D98))</f>
+        <v>79</v>
+      </c>
+      <c r="D98" t="s">
+        <v>83</v>
+      </c>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="9"/>
+      <c r="L98" s="9"/>
+      <c r="M98" s="9"/>
+      <c r="N98" s="9"/>
+      <c r="O98" s="9"/>
+      <c r="P98" s="9"/>
+      <c r="Q98" s="9"/>
+      <c r="R98" s="9"/>
+      <c r="S98" s="9"/>
+      <c r="T98" s="9"/>
+      <c r="U98" s="9"/>
+      <c r="V98" s="9"/>
+      <c r="W98" s="9"/>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <f>IF(ISBLANK(B99),"",COUNTA($B$4:B99))</f>
         <v>17</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>6</v>
       </c>
-      <c r="C98" t="str">
-        <f>IF(ISBLANK(D98),"",COUNTA($D$5:D98))</f>
-        <v/>
-      </c>
-      <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
-      <c r="K98" s="1"/>
-      <c r="L98" s="1"/>
-      <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
-      <c r="O98" s="1"/>
-      <c r="P98" s="1"/>
-      <c r="Q98" s="1"/>
-      <c r="R98" s="1"/>
-      <c r="S98" s="1"/>
-      <c r="T98" s="1"/>
-      <c r="U98" s="1"/>
-      <c r="V98" s="1"/>
-      <c r="W98" s="1"/>
-      <c r="X98" s="4"/>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="C99" t="str">
+        <f>IF(ISBLANK(D99),"",COUNTA($D$5:D99))</f>
+        <v/>
+      </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
@@ -4078,6 +4087,7 @@
       <c r="U99" s="1"/>
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
+      <c r="X99" s="4"/>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.35">
       <c r="H100" s="1"/>
@@ -4097,6 +4107,24 @@
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
     </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="F3:G3"/>

</xml_diff>

<commit_message>
Enforcing filling all trips details from modal
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624FA42F-BFE9-4FFF-9BF8-280A9A60CE30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC912471-CE01-48B2-9566-FEC68B66D060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
   <si>
     <t>June</t>
   </si>
@@ -1061,10 +1061,10 @@
   <dimension ref="A1:X101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="23" ySplit="3" topLeftCell="X40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="3" topLeftCell="X64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G87" sqref="G87"/>
+      <selection pane="bottomRight" activeCell="J45" sqref="J45:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="9"/>
+      <c r="J41" s="16"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="9"/>
+      <c r="J42" s="16"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="9"/>
+      <c r="J43" s="16"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="9"/>
+      <c r="J44" s="16"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="9"/>
+      <c r="J45" s="16"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="9"/>
+      <c r="J46" s="16"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>

</xml_diff>

<commit_message>
Enabled picture upload from profile page
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC912471-CE01-48B2-9566-FEC68B66D060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422ADFEA-289B-4DDC-832F-BD6CB191174C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="92">
   <si>
     <t>June</t>
   </si>
@@ -1061,10 +1061,10 @@
   <dimension ref="A1:X101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="23" ySplit="3" topLeftCell="X64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="3" topLeftCell="X34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J45" sqref="J45:J46"/>
+      <selection pane="bottomRight" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3293,7 +3293,7 @@
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
-      <c r="O72" s="9"/>
+      <c r="O72" s="16"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -3322,7 +3322,7 @@
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
-      <c r="O73" s="9"/>
+      <c r="O73" s="16"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
@@ -3351,7 +3351,7 @@
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
-      <c r="O74" s="9"/>
+      <c r="O74" s="16"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
@@ -3380,7 +3380,7 @@
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
-      <c r="O75" s="9"/>
+      <c r="O75" s="16"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
@@ -3409,7 +3409,7 @@
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
-      <c r="O76" s="9"/>
+      <c r="O76" s="16"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>

</xml_diff>

<commit_message>
Functioning removal of user profile and complete removal of all notifications when removing trip
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EFFDA7-41DC-4DBA-8E0C-4C6E4FC0D2C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1BB6F1-CBA8-4374-A85E-A90336B15D32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34440" windowHeight="12170" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="1030" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
   <sheets>
     <sheet name="Critical path analysis" sheetId="3" r:id="rId1"/>
@@ -1069,10 +1069,10 @@
   <dimension ref="A1:X101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="23" ySplit="3" topLeftCell="X31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O55" sqref="O55"/>
+      <selection pane="bottomRight" activeCell="P78" sqref="P78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2385,12 +2385,10 @@
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="16"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -2414,12 +2412,10 @@
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="16"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -2443,12 +2439,10 @@
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="16"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
@@ -2472,12 +2466,10 @@
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="16"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
@@ -2501,12 +2493,10 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="16"/>
       <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
@@ -2530,12 +2520,10 @@
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="16"/>
       <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
@@ -2592,13 +2580,11 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
-      <c r="K48" s="9"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
+      <c r="O48" s="15"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
@@ -2621,13 +2607,11 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
-      <c r="K49" s="9"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
+      <c r="O49" s="15"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
@@ -2650,13 +2634,11 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
-      <c r="K50" s="9"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
+      <c r="O50" s="15"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
@@ -2679,13 +2661,11 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="9"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
@@ -2708,13 +2688,11 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="9"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="O52" s="15"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
@@ -2737,13 +2715,11 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
-      <c r="K53" s="9"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
@@ -2766,13 +2742,11 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
-      <c r="K54" s="9"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
+      <c r="O54" s="15"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
@@ -2795,13 +2769,11 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
-      <c r="K55" s="9"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
@@ -2857,13 +2829,13 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="9"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
+      <c r="R57" s="15"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
@@ -2886,13 +2858,13 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
-      <c r="N58" s="9"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
+      <c r="R58" s="15"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
@@ -2915,13 +2887,13 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
-      <c r="N59" s="9"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
+      <c r="R59" s="15"/>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
@@ -2944,13 +2916,13 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
-      <c r="L60" s="9"/>
-      <c r="M60" s="9"/>
-      <c r="N60" s="9"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
+      <c r="R60" s="15"/>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
@@ -2973,13 +2945,13 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
-      <c r="N61" s="9"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
+      <c r="R61" s="15"/>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
@@ -3002,13 +2974,13 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
+      <c r="R62" s="15"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
@@ -3063,13 +3035,13 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
-      <c r="N64" s="9"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
+      <c r="R64" s="15"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
@@ -3092,13 +3064,13 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
-      <c r="L65" s="9"/>
-      <c r="M65" s="9"/>
-      <c r="N65" s="9"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
+      <c r="R65" s="15"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
@@ -3121,13 +3093,13 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
-      <c r="L66" s="9"/>
-      <c r="M66" s="9"/>
-      <c r="N66" s="9"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
+      <c r="R66" s="15"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
@@ -3150,13 +3122,13 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
+      <c r="R67" s="15"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -3179,13 +3151,13 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
-      <c r="N68" s="9"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
+      <c r="R68" s="15"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
@@ -3208,13 +3180,13 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
-      <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
+      <c r="R69" s="15"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
@@ -3237,13 +3209,13 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="9"/>
-      <c r="M70" s="9"/>
-      <c r="N70" s="9"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
+      <c r="R70" s="15"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
@@ -3296,12 +3268,11 @@
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
+      <c r="J72" s="17"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
-      <c r="O72" s="17"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -3325,12 +3296,11 @@
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
+      <c r="J73" s="17"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
-      <c r="O73" s="17"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
       <c r="R73" s="1"/>
@@ -3354,12 +3324,11 @@
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
+      <c r="J74" s="17"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
-      <c r="O74" s="17"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
@@ -3383,12 +3352,11 @@
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
+      <c r="J75" s="17"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
-      <c r="O75" s="17"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
       <c r="R75" s="1"/>
@@ -3412,12 +3380,11 @@
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
+      <c r="J76" s="17"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
-      <c r="O76" s="17"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
@@ -3441,12 +3408,11 @@
       </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
+      <c r="J77" s="15"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
-      <c r="O77" s="9"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
       <c r="R77" s="1"/>
@@ -3503,12 +3469,11 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
+      <c r="K79" s="15"/>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
-      <c r="P79" s="15"/>
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
@@ -3532,12 +3497,11 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
+      <c r="K80" s="15"/>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
-      <c r="P80" s="15"/>
       <c r="Q80" s="1"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
@@ -3561,12 +3525,11 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
+      <c r="K81" s="15"/>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
-      <c r="P81" s="15"/>
       <c r="Q81" s="1"/>
       <c r="R81" s="1"/>
       <c r="S81" s="1"/>
@@ -3590,12 +3553,11 @@
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
+      <c r="K82" s="15"/>
       <c r="L82" s="1"/>
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
-      <c r="P82" s="15"/>
       <c r="Q82" s="1"/>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
@@ -3619,12 +3581,11 @@
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
+      <c r="K83" s="15"/>
       <c r="L83" s="1"/>
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
-      <c r="P83" s="15"/>
       <c r="Q83" s="1"/>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
@@ -3648,12 +3609,11 @@
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
-      <c r="K84" s="1"/>
+      <c r="K84" s="15"/>
       <c r="L84" s="1"/>
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
-      <c r="P84" s="9"/>
       <c r="Q84" s="1"/>
       <c r="R84" s="1"/>
       <c r="S84" s="1"/>

</xml_diff>

<commit_message>
Added demo gifs to home page to demonstrate functionality when user logged out
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1BB6F1-CBA8-4374-A85E-A90336B15D32}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BE4FA1-C821-4C7B-8CC4-17C2B75711A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="1030" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -326,7 +326,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,12 +348,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -493,7 +487,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1069,10 +1062,10 @@
   <dimension ref="A1:X101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="23" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="23" ySplit="3" topLeftCell="X58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P78" sqref="P78"/>
+      <selection pane="bottomRight" activeCell="Q87" sqref="Q87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,10 +1182,10 @@
       <c r="E3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="19"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="8" t="s">
         <v>40</v>
       </c>
@@ -1205,11 +1198,11 @@
       <c r="K3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
       <c r="O3" s="8" t="s">
         <v>45</v>
       </c>
@@ -1219,21 +1212,21 @@
       <c r="Q3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="20" t="s">
+      <c r="R3" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="21"/>
-      <c r="T3" s="22"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21"/>
       <c r="U3" s="8" t="s">
         <v>49</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="W3" s="20" t="s">
+      <c r="W3" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="X3" s="22"/>
+      <c r="X3" s="21"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1667,17 +1660,17 @@
         <v>53</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="16"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1699,17 +1692,17 @@
         <v>54</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="16"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -3268,7 +3261,7 @@
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="17"/>
+      <c r="J72" s="16"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -3296,7 +3289,7 @@
       </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="17"/>
+      <c r="J73" s="16"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
@@ -3324,7 +3317,7 @@
       </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
-      <c r="J74" s="17"/>
+      <c r="J74" s="16"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -3352,7 +3345,7 @@
       </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
-      <c r="J75" s="17"/>
+      <c r="J75" s="16"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
@@ -3380,7 +3373,7 @@
       </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
-      <c r="J76" s="17"/>
+      <c r="J76" s="16"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>

</xml_diff>

<commit_message>
Fixed unit test for authentication after changing sameSite attribute. Continued writing report - WIP implementation
</commit_message>
<xml_diff>
--- a/docs/preliminary_report/planning/Gantt chart.xlsx
+++ b/docs/preliminary_report/planning/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventafri\Desktop\Uni\year 3\UniFinalProject\docs\preliminary_report\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BE4FA1-C821-4C7B-8CC4-17C2B75711A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6590E053-C14C-49CB-AD50-EFBA90538C57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="1030" activeTab="1" xr2:uid="{2CF04310-1528-4712-A49B-94228FE17A40}"/>
   </bookViews>
@@ -1065,7 +1065,7 @@
       <pane xSplit="23" ySplit="3" topLeftCell="X58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="X1" sqref="X1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q87" sqref="Q87"/>
+      <selection pane="bottomRight" activeCell="V93" sqref="V93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3694,8 +3694,8 @@
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
       <c r="P87" s="1"/>
-      <c r="Q87" s="9"/>
-      <c r="R87" s="1"/>
+      <c r="Q87" s="15"/>
+      <c r="R87" s="15"/>
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
@@ -3952,11 +3952,11 @@
       <c r="P96" s="1"/>
       <c r="Q96" s="1"/>
       <c r="R96" s="1"/>
-      <c r="S96" s="1"/>
-      <c r="T96" s="1"/>
-      <c r="U96" s="9"/>
-      <c r="V96" s="9"/>
-      <c r="W96" s="9"/>
+      <c r="S96" s="15"/>
+      <c r="T96" s="15"/>
+      <c r="U96" s="15"/>
+      <c r="V96" s="15"/>
+      <c r="W96" s="15"/>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A97" t="str">
@@ -3983,9 +3983,9 @@
       <c r="R97" s="1"/>
       <c r="S97" s="1"/>
       <c r="T97" s="1"/>
-      <c r="U97" s="9"/>
-      <c r="V97" s="9"/>
-      <c r="W97" s="9"/>
+      <c r="U97" s="15"/>
+      <c r="V97" s="15"/>
+      <c r="W97" s="15"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A98" t="str">
@@ -3999,25 +3999,25 @@
       <c r="D98" t="s">
         <v>83</v>
       </c>
-      <c r="E98" s="9"/>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
-      <c r="I98" s="9"/>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-      <c r="M98" s="9"/>
-      <c r="N98" s="9"/>
-      <c r="O98" s="9"/>
-      <c r="P98" s="9"/>
-      <c r="Q98" s="9"/>
-      <c r="R98" s="9"/>
-      <c r="S98" s="9"/>
-      <c r="T98" s="9"/>
-      <c r="U98" s="9"/>
-      <c r="V98" s="9"/>
-      <c r="W98" s="9"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="15"/>
+      <c r="L98" s="15"/>
+      <c r="M98" s="15"/>
+      <c r="N98" s="15"/>
+      <c r="O98" s="15"/>
+      <c r="P98" s="15"/>
+      <c r="Q98" s="15"/>
+      <c r="R98" s="15"/>
+      <c r="S98" s="15"/>
+      <c r="T98" s="15"/>
+      <c r="U98" s="15"/>
+      <c r="V98" s="15"/>
+      <c r="W98" s="15"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A99">

</xml_diff>